<commit_message>
Simulation Graphs added distance
Change-Id: I0af42d3cc7f8f26565c3b0bba24aa96b60a3a397
Signed-off-by: Andrey Shamis <lolnik@gmail.com>
</commit_message>
<xml_diff>
--- a/Results/For Presentation/Graphs.xlsx
+++ b/Results/For Presentation/Graphs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t>BSS</t>
   </si>
@@ -50,6 +50,15 @@
   <si>
     <t>Speed Mbs</t>
   </si>
+  <si>
+    <t>STA 1</t>
+  </si>
+  <si>
+    <t>STA 2</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
 </sst>
 </file>
 
@@ -73,7 +82,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,12 +90,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1104,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D22" sqref="A19:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,6 +1281,114 @@
       </c>
       <c r="D16">
         <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>50</v>
+      </c>
+      <c r="D20" s="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>50</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1">
+        <v>55</v>
+      </c>
+      <c r="C22" s="1">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>92</v>
+      </c>
+      <c r="D26" s="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="1">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1">
+        <v>93</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>